<commit_message>
salvando a partir da máquina da empresa
</commit_message>
<xml_diff>
--- a/project/0_rts/RT2604/1-Referências Técnicas/Planilha_Abaco_Gooseneck_MCV_Global_10k_MUX-Rev8.xlsx
+++ b/project/0_rts/RT2604/1-Referências Técnicas/Planilha_Abaco_Gooseneck_MCV_Global_10k_MUX-Rev8.xlsx
@@ -5370,11 +5370,10 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e22693a2-11d8-4e06-9932-42f8499655b9">
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="461c5b05-e7ae-45a9-96d4-4a689e060405">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7240fca1-d5d8-4b7d-af8f-d58b11c87bd0" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="e22693a2-11d8-4e06-9932-42f8499655b9" xsi:nil="true"/>
+    <TaxCatchAll xmlns="903036b2-f8dc-4ca8-82df-457cf2fff651" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
@@ -5389,10 +5388,11 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002E90C87AC8820043BFE71A5FB0DDB6EC" ma:contentTypeVersion="15" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="a2a8ce1f5bc7a9ae8b5abdcb00b6cafe">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e22693a2-11d8-4e06-9932-42f8499655b9" xmlns:ns3="7240fca1-d5d8-4b7d-af8f-d58b11c87bd0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b146a6bcd0f4c9724cf477ac809c65e8" ns2:_="" ns3:_="">
-    <xsd:import namespace="e22693a2-11d8-4e06-9932-42f8499655b9"/>
-    <xsd:import namespace="7240fca1-d5d8-4b7d-af8f-d58b11c87bd0"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010069E487C1B5A6A7469ECF295E300FC521" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="0960ac6fc61b40489ab078022ce7de8d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="509bbd28-9a6d-445a-83dd-f5d328eece76" xmlns:ns3="903036b2-f8dc-4ca8-82df-457cf2fff651" xmlns:ns4="461c5b05-e7ae-45a9-96d4-4a689e060405" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d2f069df8fef6df821bd87bc04dd1b2c" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="509bbd28-9a6d-445a-83dd-f5d328eece76"/>
+    <xsd:import namespace="903036b2-f8dc-4ca8-82df-457cf2fff651"/>
+    <xsd:import namespace="461c5b05-e7ae-45a9-96d4-4a689e060405"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -5401,18 +5401,18 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:_Flow_SignoffStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns4:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5420,7 +5420,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e22693a2-11d8-4e06-9932-42f8499655b9" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="509bbd28-9a6d-445a-83dd-f5d328eece76" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -5433,71 +5433,11 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5103c4ab-04ed-4a1f-bb47-9362306674cb" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="13" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="20" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="_Flow_SignoffStatus" ma:index="21" nillable="true" ma:displayName="Sign-off status" ma:internalName="Sign_x002d_off_x0020_status">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7240fca1-d5d8-4b7d-af8f-d58b11c87bd0" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="903036b2-f8dc-4ca8-82df-457cf2fff651" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="12" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{12529d39-6b3f-49f3-8254-0ddaa0523a13}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7240fca1-d5d8-4b7d-af8f-d58b11c87bd0">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Compartilhado com" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Compartilhado com" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -5516,11 +5456,75 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{671d7225-7c32-4489-b6da-c381a375bb6a}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="903036b2-f8dc-4ca8-82df-457cf2fff651">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="461c5b05-e7ae-45a9-96d4-4a689e060405" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5103c4ab-04ed-4a1f-bb47-9362306674cb" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="20" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -5632,5 +5636,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32202815-5895-48AC-A81A-A5F909FAE364}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD5C3B4-F38D-45DF-9922-5C4AAC071947}"/>
 </file>
</xml_diff>